<commit_message>
added pcos sys review test results
</commit_message>
<xml_diff>
--- a/demo/testing_pcos_sys_review.xlsx
+++ b/demo/testing_pcos_sys_review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darre\Documents\Second-Brain\4 Jupyter Notebooks\evidence_synthesis_automation_labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darre\Documents\GitHub\handsearch_test\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B416CD8-D1D2-40D6-A460-3EAFC1D5E68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E9542-DBB6-427A-82FE-0923E0E5F7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="300" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{0088CB58-4EED-4220-909D-CFD71481CABD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0088CB58-4EED-4220-909D-CFD71481CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Run</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Development and Psychometric Properties of the Female Sexual Desire Questionnaire (FSDQ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recall </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieved Paper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Included </t>
   </si>
 </sst>
 </file>
@@ -585,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEF1517-AA97-44D2-85F5-3EF6E14FA5E9}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +611,7 @@
     <col min="4" max="4" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -618,12 +630,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -636,8 +648,11 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>27.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -647,30 +662,46 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>10*(0.8667)</f>
+        <v>8.6669999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>20*(0.92)</f>
+        <v>18.400000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>35*0.78</f>
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>B6*B7*B8</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>SUM(G5:G8)</f>
+        <v>82.227000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -678,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -687,14 +718,43 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f>D21/C21</f>
+        <v>9.3506493506493506E-3</v>
+      </c>
+      <c r="C21">
+        <v>1925</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -812,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7D4DB2-CD2C-482F-9361-F991FF1F0C7E}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>